<commit_message>
change to semicolon separators
</commit_message>
<xml_diff>
--- a/PowerWashSimulator/data.xlsx
+++ b/PowerWashSimulator/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubChelsea\HadesGame-Checklist\PowerWashSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8F378D-E1F9-4145-AB30-C2E15CA118D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D79D20-27A6-4F5B-AADB-73122FBC2BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30C4C3A8-F402-46FC-A1A0-0B0F8647869F}"/>
   </bookViews>
@@ -991,7 +991,7 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
style and data update
</commit_message>
<xml_diff>
--- a/PowerWashSimulator/data.xlsx
+++ b/PowerWashSimulator/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubChelsea\HadesGame-Checklist\PowerWashSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D79D20-27A6-4F5B-AADB-73122FBC2BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2835A7-1473-40F9-AF83-867057041CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30C4C3A8-F402-46FC-A1A0-0B0F8647869F}"/>
   </bookViews>
@@ -628,12 +628,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -648,12 +654,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BEB57F3-4A37-4B35-911F-04B3CFC91EFD}">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,13 +1473,16 @@
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
@@ -1661,13 +1671,16 @@
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
       <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
         <v>1</v>
       </c>
     </row>
@@ -1858,8 +1871,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B33" t="s">
@@ -1868,9 +1881,12 @@
       <c r="C33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B34" t="s">
@@ -1879,8 +1895,11 @@
       <c r="C34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -1891,7 +1910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -1902,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1913,7 +1932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -1924,7 +1943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -1935,7 +1954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -1946,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>

</xml_diff>